<commit_message>
Updated tagLookup with new tags
</commit_message>
<xml_diff>
--- a/lookups/20200611 tagLookup.xlsx
+++ b/lookups/20200611 tagLookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Evidence\DMBI\Care Opinion\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Evidence\DMBI\Care Opinion\careopinionstoryboard\lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29920413-E1C2-42C4-80F2-DBDEC10CED48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F80C87-17A5-4D38-AAF9-00DE44D7500B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tagLookup" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="1843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1846">
   <si>
     <t>tagName</t>
   </si>
@@ -5494,84 +5494,97 @@
     <t>Willingness to help</t>
   </si>
   <si>
+    <t>Access to bed</t>
+  </si>
+  <si>
+    <t>Not helped</t>
+  </si>
+  <si>
+    <t>Communciation</t>
+  </si>
+  <si>
+    <t>Thoroughness</t>
+  </si>
+  <si>
+    <t>Cold waiting area</t>
+  </si>
+  <si>
+    <t>Lost property</t>
+  </si>
+  <si>
+    <t>Questions not answered</t>
+  </si>
+  <si>
+    <t>Wrong information</t>
+  </si>
+  <si>
+    <t>Family care</t>
+  </si>
+  <si>
+    <t>Hurtful comments</t>
+  </si>
+  <si>
+    <t>Internet access</t>
+  </si>
+  <si>
+    <t>Medication administration</t>
+  </si>
+  <si>
+    <t>Mental health help</t>
+  </si>
+  <si>
+    <t>More space</t>
+  </si>
+  <si>
+    <t>One doctor</t>
+  </si>
+  <si>
+    <t>Phoneline</t>
+  </si>
+  <si>
+    <t>Regular checks</t>
+  </si>
+  <si>
+    <t>Scans</t>
+  </si>
+  <si>
+    <t>Side effects</t>
+  </si>
+  <si>
+    <t>Spoken down to</t>
+  </si>
+  <si>
+    <t>Time wasting</t>
+  </si>
+  <si>
+    <t>Undignified</t>
+  </si>
+  <si>
+    <t>Voicemail</t>
+  </si>
+  <si>
+    <t>Car Parking</t>
+  </si>
+  <si>
+    <t>Lack of compassion</t>
+  </si>
+  <si>
     <t>These codes are for classifying comments about peoples experience of care. Leave blank anything that's:
-- about the persons health condition
-- an emotion tag
-- too vague to classifiy (e.g. "Investigations")
+- about: 
+   - emotion, 
+   - condition, 
+   - cause of disease, or
+   - parts of body  - these should be filtered out
+- too vague to classifiy (e.g. "Investigations"), or
 - the name of a service
-Try to use the most specific code or altenatively the group code (in CAPS).</t>
-  </si>
-  <si>
-    <t>Access to bed</t>
-  </si>
-  <si>
-    <t>Not helped</t>
-  </si>
-  <si>
-    <t>Communciation</t>
-  </si>
-  <si>
-    <t>Thoroughness</t>
-  </si>
-  <si>
-    <t>Cold waiting area</t>
-  </si>
-  <si>
-    <t>Lost property</t>
-  </si>
-  <si>
-    <t>Questions not answered</t>
-  </si>
-  <si>
-    <t>Wrong information</t>
-  </si>
-  <si>
-    <t>Family care</t>
-  </si>
-  <si>
-    <t>Hurtful comments</t>
-  </si>
-  <si>
-    <t>Internet access</t>
-  </si>
-  <si>
-    <t>Medication administration</t>
-  </si>
-  <si>
-    <t>Mental health help</t>
-  </si>
-  <si>
-    <t>More space</t>
-  </si>
-  <si>
-    <t>One doctor</t>
-  </si>
-  <si>
-    <t>Phoneline</t>
-  </si>
-  <si>
-    <t>Regular checks</t>
-  </si>
-  <si>
-    <t>Scans</t>
-  </si>
-  <si>
-    <t>Side effects</t>
-  </si>
-  <si>
-    <t>Spoken down to</t>
-  </si>
-  <si>
-    <t>Time wasting</t>
-  </si>
-  <si>
-    <t>Undignified</t>
-  </si>
-  <si>
-    <t>Voicemail</t>
-  </si>
-  <si>
-    <t>Car Parking</t>
+Try to use the most specific code or altenatively the group code (in CAPS).
+tagName is not case sensitive (the R code cleans this up)</t>
+  </si>
+  <si>
+    <t>Health and safety</t>
+  </si>
+  <si>
+    <t>Mixed messages</t>
   </si>
 </sst>
 </file>
@@ -6398,11 +6411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1752"/>
+  <dimension ref="A1:D1755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1719" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1756" sqref="D1756"/>
+      <pane ySplit="1" topLeftCell="A1725" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6609,10 +6622,14 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="C17" t="s">
-        <v>832</v>
+        <v>439</v>
+      </c>
+      <c r="D17" t="str">
+        <f>IFERROR(VLOOKUP(C17,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Systems and processes</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6689,11 +6706,11 @@
         <v>533</v>
       </c>
       <c r="C24" t="s">
-        <v>510</v>
+        <v>1081</v>
       </c>
       <c r="D24" t="str">
         <f>IFERROR(VLOOKUP(C24,orderedtags!B:C,2,FALSE),"")</f>
-        <v>Staff</v>
+        <v>Access to services</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -6712,9 +6729,12 @@
       <c r="A26" t="s">
         <v>1526</v>
       </c>
+      <c r="C26" t="s">
+        <v>1081</v>
+      </c>
       <c r="D26" t="str">
         <f>IFERROR(VLOOKUP(C26,orderedtags!B:C,2,FALSE),"")</f>
-        <v/>
+        <v>Access to services</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -6794,11 +6814,11 @@
         <v>459</v>
       </c>
       <c r="C33" t="s">
-        <v>439</v>
+        <v>1081</v>
       </c>
       <c r="D33" t="str">
         <f>IFERROR(VLOOKUP(C33,orderedtags!B:C,2,FALSE),"")</f>
-        <v>Systems and processes</v>
+        <v>Access to services</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -6842,11 +6862,11 @@
         <v>1170</v>
       </c>
       <c r="C37" t="s">
-        <v>1081</v>
+        <v>646</v>
       </c>
       <c r="D37" t="str">
         <f>IFERROR(VLOOKUP(C37,orderedtags!B:C,2,FALSE),"")</f>
-        <v>Access to services</v>
+        <v>Clincal care</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -7022,11 +7042,11 @@
         <v>1336</v>
       </c>
       <c r="C52" t="s">
-        <v>1081</v>
+        <v>932</v>
       </c>
       <c r="D52" t="str">
         <f>IFERROR(VLOOKUP(C52,orderedtags!B:C,2,FALSE),"")</f>
-        <v>Access to services</v>
+        <v>Clincal care</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -8578,6 +8598,10 @@
       <c r="A184" t="s">
         <v>754</v>
       </c>
+      <c r="D184" t="str">
+        <f>IFERROR(VLOOKUP(C184,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
@@ -9228,6 +9252,10 @@
       <c r="A239" t="s">
         <v>70</v>
       </c>
+      <c r="D239" t="str">
+        <f>IFERROR(VLOOKUP(C239,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
@@ -9719,9 +9747,12 @@
       <c r="A281" t="s">
         <v>1683</v>
       </c>
+      <c r="C281" t="s">
+        <v>1056</v>
+      </c>
       <c r="D281" t="str">
         <f>IFERROR(VLOOKUP(C281,orderedtags!B:C,2,FALSE),"")</f>
-        <v/>
+        <v>Care</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -9939,7 +9970,14 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>1823</v>
+        <v>1822</v>
+      </c>
+      <c r="C300" t="s">
+        <v>832</v>
+      </c>
+      <c r="D300" t="str">
+        <f>IFERROR(VLOOKUP(C300,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Environment and Facilities</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -9973,6 +10011,10 @@
       <c r="B303">
         <v>1</v>
       </c>
+      <c r="D303" t="str">
+        <f>IFERROR(VLOOKUP(C303,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
@@ -10012,7 +10054,14 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>1821</v>
+        <v>1820</v>
+      </c>
+      <c r="C307" t="s">
+        <v>96</v>
+      </c>
+      <c r="D307" t="str">
+        <f>IFERROR(VLOOKUP(C307,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Communication and information</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -12545,9 +12594,12 @@
       <c r="A519" t="s">
         <v>1673</v>
       </c>
+      <c r="C519" t="s">
+        <v>738</v>
+      </c>
       <c r="D519" t="str">
         <f>IFERROR(VLOOKUP(C519,orderedtags!B:C,2,FALSE),"")</f>
-        <v/>
+        <v>General</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
@@ -12753,7 +12805,11 @@
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1827</v>
+        <v>1826</v>
+      </c>
+      <c r="D537" t="str">
+        <f>IFERROR(VLOOKUP(C537,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
@@ -14386,10 +14442,18 @@
       <c r="A675" t="s">
         <v>764</v>
       </c>
+      <c r="D675" t="str">
+        <f>IFERROR(VLOOKUP(C675,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="676" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>1828</v>
+        <v>1827</v>
+      </c>
+      <c r="D676" t="str">
+        <f>IFERROR(VLOOKUP(C676,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="677" spans="1:4" x14ac:dyDescent="0.25">
@@ -14588,6 +14652,10 @@
       <c r="A693" t="s">
         <v>1185</v>
       </c>
+      <c r="D693" t="str">
+        <f>IFERROR(VLOOKUP(C693,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="694" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
@@ -15058,6 +15126,10 @@
       <c r="B733">
         <v>1</v>
       </c>
+      <c r="D733" t="str">
+        <f>IFERROR(VLOOKUP(C733,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="734" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
@@ -15208,7 +15280,11 @@
     </row>
     <row r="747" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1829</v>
+        <v>1828</v>
+      </c>
+      <c r="D747" t="str">
+        <f>IFERROR(VLOOKUP(C747,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="748" spans="1:4" x14ac:dyDescent="0.25">
@@ -15500,6 +15576,10 @@
       <c r="A772" t="s">
         <v>903</v>
       </c>
+      <c r="D772" t="str">
+        <f>IFERROR(VLOOKUP(C772,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="773" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
@@ -15604,6 +15684,10 @@
       <c r="A781" t="s">
         <v>1540</v>
       </c>
+      <c r="D781" t="str">
+        <f>IFERROR(VLOOKUP(C781,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="782" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
@@ -16035,6 +16119,10 @@
       <c r="A818" t="s">
         <v>900</v>
       </c>
+      <c r="D818" t="str">
+        <f>IFERROR(VLOOKUP(C818,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
@@ -16145,6 +16233,10 @@
       <c r="A828" t="s">
         <v>223</v>
       </c>
+      <c r="D828" t="str">
+        <f>IFERROR(VLOOKUP(C828,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
@@ -16409,7 +16501,14 @@
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>1824</v>
+        <v>1823</v>
+      </c>
+      <c r="C851" t="s">
+        <v>610</v>
+      </c>
+      <c r="D851" t="str">
+        <f>IFERROR(VLOOKUP(C851,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Person centred care</v>
       </c>
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.25">
@@ -16744,7 +16843,11 @@
     </row>
     <row r="880" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
-        <v>1830</v>
+        <v>1829</v>
+      </c>
+      <c r="D880" t="str">
+        <f>IFERROR(VLOOKUP(C880,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="881" spans="1:4" x14ac:dyDescent="0.25">
@@ -16893,7 +16996,11 @@
     </row>
     <row r="893" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>1831</v>
+        <v>1830</v>
+      </c>
+      <c r="D893" t="str">
+        <f>IFERROR(VLOOKUP(C893,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="894" spans="1:4" x14ac:dyDescent="0.25">
@@ -17029,6 +17136,10 @@
       <c r="A905" t="s">
         <v>686</v>
       </c>
+      <c r="D905" t="str">
+        <f>IFERROR(VLOOKUP(C905,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="906" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
@@ -17464,7 +17575,11 @@
     </row>
     <row r="943" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A943" t="s">
-        <v>1832</v>
+        <v>1831</v>
+      </c>
+      <c r="D943" t="str">
+        <f>IFERROR(VLOOKUP(C943,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="944" spans="1:4" x14ac:dyDescent="0.25">
@@ -18183,10 +18298,14 @@
     </row>
     <row r="1004" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1004" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="C1004" t="s">
         <v>1081</v>
+      </c>
+      <c r="D1004" t="str">
+        <f>IFERROR(VLOOKUP(C1004,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Access to services</v>
       </c>
     </row>
     <row r="1005" spans="1:4" x14ac:dyDescent="0.25">
@@ -18229,6 +18348,10 @@
       <c r="A1008" t="s">
         <v>253</v>
       </c>
+      <c r="D1008" t="str">
+        <f>IFERROR(VLOOKUP(C1008,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1009" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
@@ -18529,7 +18652,11 @@
     </row>
     <row r="1034" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
-        <v>1833</v>
+        <v>1832</v>
+      </c>
+      <c r="D1034" t="str">
+        <f>IFERROR(VLOOKUP(C1034,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1035" spans="1:4" x14ac:dyDescent="0.25">
@@ -19622,6 +19749,10 @@
       <c r="B1126">
         <v>-1</v>
       </c>
+      <c r="D1126" t="str">
+        <f>IFERROR(VLOOKUP(C1126,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1127" t="s">
@@ -19958,7 +20089,14 @@
     </row>
     <row r="1155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1155" t="s">
-        <v>1834</v>
+        <v>1833</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>598</v>
+      </c>
+      <c r="D1155" t="str">
+        <f>IFERROR(VLOOKUP(C1155,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Phone calls</v>
       </c>
     </row>
     <row r="1156" spans="1:4" x14ac:dyDescent="0.25">
@@ -20848,7 +20986,7 @@
         <v>683</v>
       </c>
       <c r="C1232" t="s">
-        <v>681</v>
+        <v>960</v>
       </c>
       <c r="D1232" t="str">
         <f>IFERROR(VLOOKUP(C1232,orderedtags!B:C,2,FALSE),"")</f>
@@ -20857,7 +20995,14 @@
     </row>
     <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1233" t="s">
-        <v>1825</v>
+        <v>1824</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>960</v>
+      </c>
+      <c r="D1233" t="str">
+        <f>IFERROR(VLOOKUP(C1233,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Communication and information</v>
       </c>
     </row>
     <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
@@ -21396,7 +21541,11 @@
     </row>
     <row r="1279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1279" t="s">
-        <v>1835</v>
+        <v>1834</v>
+      </c>
+      <c r="D1279" t="str">
+        <f>IFERROR(VLOOKUP(C1279,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1280" spans="1:4" x14ac:dyDescent="0.25">
@@ -21787,9 +21936,12 @@
       <c r="A1313" t="s">
         <v>1255</v>
       </c>
+      <c r="C1313" t="s">
+        <v>1058</v>
+      </c>
       <c r="D1313" t="str">
         <f>IFERROR(VLOOKUP(C1313,orderedtags!B:C,2,FALSE),"")</f>
-        <v/>
+        <v>Assessment and management</v>
       </c>
     </row>
     <row r="1314" spans="1:4" x14ac:dyDescent="0.25">
@@ -22079,7 +22231,11 @@
     </row>
     <row r="1338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1338" t="s">
-        <v>1836</v>
+        <v>1835</v>
+      </c>
+      <c r="D1338" t="str">
+        <f>IFERROR(VLOOKUP(C1338,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1339" spans="1:4" x14ac:dyDescent="0.25">
@@ -22483,7 +22639,14 @@
     </row>
     <row r="1374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1374" t="s">
-        <v>1837</v>
+        <v>1836</v>
+      </c>
+      <c r="C1374" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1374" t="str">
+        <f>IFERROR(VLOOKUP(C1374,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Clincal care</v>
       </c>
     </row>
     <row r="1375" spans="1:4" x14ac:dyDescent="0.25">
@@ -22679,6 +22842,13 @@
       <c r="A1391" t="s">
         <v>1653</v>
       </c>
+      <c r="C1391" t="s">
+        <v>738</v>
+      </c>
+      <c r="D1391" t="str">
+        <f>IFERROR(VLOOKUP(C1391,orderedtags!B:C,2,FALSE),"")</f>
+        <v>General</v>
+      </c>
     </row>
     <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1392" t="s">
@@ -22889,7 +23059,11 @@
     </row>
     <row r="1410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1410" t="s">
-        <v>1838</v>
+        <v>1837</v>
+      </c>
+      <c r="D1410" t="str">
+        <f>IFERROR(VLOOKUP(C1410,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1411" spans="1:4" x14ac:dyDescent="0.25">
@@ -23400,9 +23574,12 @@
       <c r="B1454">
         <v>-1</v>
       </c>
+      <c r="C1454" t="s">
+        <v>738</v>
+      </c>
       <c r="D1454" t="str">
         <f>IFERROR(VLOOKUP(C1454,orderedtags!B:C,2,FALSE),"")</f>
-        <v/>
+        <v>General</v>
       </c>
     </row>
     <row r="1455" spans="1:4" x14ac:dyDescent="0.25">
@@ -23421,6 +23598,10 @@
       <c r="A1456" t="s">
         <v>755</v>
       </c>
+      <c r="D1456" t="str">
+        <f>IFERROR(VLOOKUP(C1456,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1457" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1457" t="s">
@@ -23768,6 +23949,10 @@
       <c r="A1486" t="s">
         <v>339</v>
       </c>
+      <c r="D1486" t="str">
+        <f>IFERROR(VLOOKUP(C1486,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1487" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1487" t="s">
@@ -24188,7 +24373,14 @@
     </row>
     <row r="1522" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1522" t="s">
-        <v>1822</v>
+        <v>1821</v>
+      </c>
+      <c r="C1522" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D1522" t="str">
+        <f>IFERROR(VLOOKUP(C1522,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Care</v>
       </c>
     </row>
     <row r="1523" spans="1:4" x14ac:dyDescent="0.25">
@@ -24334,7 +24526,11 @@
     </row>
     <row r="1535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1535" t="s">
-        <v>1839</v>
+        <v>1838</v>
+      </c>
+      <c r="D1535" t="str">
+        <f>IFERROR(VLOOKUP(C1535,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1536" spans="1:4" x14ac:dyDescent="0.25">
@@ -24410,6 +24606,10 @@
       <c r="A1542" t="s">
         <v>744</v>
       </c>
+      <c r="D1542" t="str">
+        <f>IFERROR(VLOOKUP(C1542,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1543" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1543" t="s">
@@ -24727,6 +24927,13 @@
       <c r="B1569">
         <v>-1</v>
       </c>
+      <c r="C1569" t="s">
+        <v>738</v>
+      </c>
+      <c r="D1569" t="str">
+        <f>IFERROR(VLOOKUP(C1569,orderedtags!B:C,2,FALSE),"")</f>
+        <v>General</v>
+      </c>
     </row>
     <row r="1570" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1570" t="s">
@@ -25101,6 +25308,10 @@
       <c r="A1601" t="s">
         <v>1591</v>
       </c>
+      <c r="D1601" t="str">
+        <f>IFERROR(VLOOKUP(C1601,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1602" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1602" t="s">
@@ -25296,7 +25507,11 @@
     </row>
     <row r="1618" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1618" t="s">
-        <v>1840</v>
+        <v>1839</v>
+      </c>
+      <c r="D1618" t="str">
+        <f>IFERROR(VLOOKUP(C1618,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1619" spans="1:4" x14ac:dyDescent="0.25">
@@ -25360,6 +25575,10 @@
       <c r="A1624" t="s">
         <v>682</v>
       </c>
+      <c r="D1624" t="str">
+        <f>IFERROR(VLOOKUP(C1624,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1625" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1625" t="s">
@@ -25527,6 +25746,10 @@
       <c r="A1639" t="s">
         <v>658</v>
       </c>
+      <c r="D1639" t="str">
+        <f>IFERROR(VLOOKUP(C1639,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1640" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1640" t="s">
@@ -25781,6 +26004,10 @@
       <c r="A1661" t="s">
         <v>1606</v>
       </c>
+      <c r="D1661" t="str">
+        <f>IFERROR(VLOOKUP(C1661,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1662" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1662" t="s">
@@ -25801,6 +26028,10 @@
       <c r="B1663">
         <v>1</v>
       </c>
+      <c r="D1663" t="str">
+        <f>IFERROR(VLOOKUP(C1663,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1664" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1664" t="s">
@@ -25809,6 +26040,10 @@
       <c r="B1664">
         <v>-1</v>
       </c>
+      <c r="D1664" t="str">
+        <f>IFERROR(VLOOKUP(C1664,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1665" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1665" t="s">
@@ -25956,7 +26191,11 @@
     </row>
     <row r="1677" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1677" t="s">
-        <v>1841</v>
+        <v>1840</v>
+      </c>
+      <c r="D1677" t="str">
+        <f>IFERROR(VLOOKUP(C1677,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1678" spans="1:4" x14ac:dyDescent="0.25">
@@ -26347,6 +26586,10 @@
       <c r="A1710" t="s">
         <v>1661</v>
       </c>
+      <c r="D1710" t="str">
+        <f>IFERROR(VLOOKUP(C1710,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1711" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1711" t="s">
@@ -26550,11 +26793,19 @@
       <c r="A1728" t="s">
         <v>386</v>
       </c>
+      <c r="D1728" t="str">
+        <f>IFERROR(VLOOKUP(C1728,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1729" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1729" t="s">
         <v>387</v>
       </c>
+      <c r="D1729" t="str">
+        <f>IFERROR(VLOOKUP(C1729,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="1730" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1730" t="s">
@@ -26762,7 +27013,11 @@
     </row>
     <row r="1747" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1747" t="s">
-        <v>1826</v>
+        <v>1825</v>
+      </c>
+      <c r="D1747" t="str">
+        <f>IFERROR(VLOOKUP(C1747,orderedtags!B:C,2,FALSE),"")</f>
+        <v/>
       </c>
     </row>
     <row r="1748" spans="1:4" x14ac:dyDescent="0.25">
@@ -26815,7 +27070,7 @@
     </row>
     <row r="1752" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1752" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="C1752" t="s">
         <v>641</v>
@@ -26823,6 +27078,42 @@
       <c r="D1752" t="str">
         <f>IFERROR(VLOOKUP(C1752,orderedtags!B:C,2,FALSE),"")</f>
         <v>Environment and Facilities</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1753" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>942</v>
+      </c>
+      <c r="D1753" t="str">
+        <f>IFERROR(VLOOKUP(C1753,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Professionalism and expertise</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1754" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1754" t="str">
+        <f>IFERROR(VLOOKUP(C1754,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Safety</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1755" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>951</v>
+      </c>
+      <c r="D1755" t="str">
+        <f>IFERROR(VLOOKUP(C1755,orderedtags!B:C,2,FALSE),"")</f>
+        <v>Communication and information</v>
       </c>
     </row>
   </sheetData>
@@ -26831,7 +27122,7 @@
       <sortCondition ref="A1:A1751"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1665:A1775">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1665:A1757">
     <sortCondition ref="A1665"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
@@ -27695,7 +27986,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27710,7 +28001,7 @@
     </row>
     <row r="2" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1818</v>
+        <v>1843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>